<commit_message>
Enhance pattern parsing and evaluation functions with new grouping logic and improved variable handling
</commit_message>
<xml_diff>
--- a/tesi/common_patterns.xlsx
+++ b/tesi/common_patterns.xlsx
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Exemple</t>
+          <t>Pattern</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -470,51 +470,51 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>0.667</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0</v>
+        <v>0.22</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AAATATATAT</t>
+          <t>ATATATAAAT</t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>1.667</v>
       </c>
       <c r="D3" t="n">
         <v>1</v>
       </c>
       <c r="E3" t="n">
-        <v>1</v>
+        <v>1.22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ATATATAAAT</t>
+          <t>AAATATATAT</t>
         </is>
       </c>
       <c r="B4" t="n">
         <v>1</v>
       </c>
       <c r="C4" t="n">
-        <v>1</v>
+        <v>1.667</v>
       </c>
       <c r="D4" t="n">
         <v>1</v>
       </c>
       <c r="E4" t="n">
-        <v>1</v>
+        <v>1.22</v>
       </c>
     </row>
     <row r="5">
@@ -546,13 +546,13 @@
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>3</v>
+        <v>3.667</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>1.33</v>
+        <v>1.56</v>
       </c>
     </row>
     <row r="7">
@@ -584,29 +584,29 @@
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>2</v>
+        <v>2.667</v>
       </c>
       <c r="D8" t="n">
         <v>2</v>
       </c>
       <c r="E8" t="n">
-        <v>2</v>
+        <v>2.22</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ATATAATAAT</t>
+          <t>ATATAAAAAT</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>2</v>
       </c>
       <c r="C9" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E9" t="n">
         <v>2.33</v>
@@ -634,17 +634,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>TAATATAAAT</t>
+          <t>ATATAATAAT</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>2</v>
       </c>
       <c r="C11" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>2.33</v>
@@ -653,36 +653,36 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ATATAAAAAT</t>
+          <t>TAATATAAAT</t>
         </is>
       </c>
       <c r="B12" t="n">
         <v>2</v>
       </c>
       <c r="C12" t="n">
-        <v>3</v>
+        <v>4.667</v>
       </c>
       <c r="D12" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" t="n">
-        <v>2.33</v>
+        <v>2.56</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>AAAAATATAT</t>
+          <t>TAATAAATAT</t>
         </is>
       </c>
       <c r="B13" t="n">
         <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D13" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
         <v>2.67</v>
@@ -691,7 +691,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ATAAATAAAT</t>
+          <t>AAAAATATAT</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -710,17 +710,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>TAATAAATAT</t>
+          <t>ATAAATAAAT</t>
         </is>
       </c>
       <c r="B15" t="n">
         <v>2</v>
       </c>
       <c r="C15" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" t="n">
         <v>2.67</v>
@@ -805,17 +805,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>AAAAATAAAT</t>
+          <t>TAATAAAAAT</t>
         </is>
       </c>
       <c r="B20" t="n">
         <v>3</v>
       </c>
       <c r="C20" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D20" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20" t="n">
         <v>3.67</v>
@@ -824,17 +824,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>TAATAAAAAT</t>
+          <t>AAAAATAAAT</t>
         </is>
       </c>
       <c r="B21" t="n">
         <v>3</v>
       </c>
       <c r="C21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D21" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E21" t="n">
         <v>3.67</v>

</xml_diff>